<commit_message>
chuc nang Ai l2
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA_SE347\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1863A7BF-D2F8-45B2-850B-AFE955F1A473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CA582F-A96E-4188-907E-FE72A2B924E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AC4B7EBD-1C64-44F2-983D-C57CA98A33B1}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -173,9 +174,6 @@
     <t>Bóp viết - Hộp bút</t>
   </si>
   <si>
-    <t>Bài - File hồ sơ</t>
-  </si>
-  <si>
     <t>Đồ bấm kim</t>
   </si>
   <si>
@@ -213,6 +211,9 @@
   </si>
   <si>
     <t>Tuổi; Năm xuất bản; Thương hiệu; Xuất sứ thương hiệu; Nơi gia công &amp; sản xuất; Màu sắc; Chất liệu ; Thông số kỹ thuật; Thông tin cảnh báo; Hướng dẫn sử dụng; Trọng lượng (gr)</t>
+  </si>
+  <si>
+    <t>Bìa - File hồ sơ</t>
   </si>
 </sst>
 </file>
@@ -586,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDFDFFD-11BC-4311-B8F4-14BBD6741A49}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -605,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -613,7 +614,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -621,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -629,7 +630,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -962,7 +963,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
         <v>36</v>
@@ -970,7 +971,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47" t="s">
         <v>36</v>
@@ -978,7 +979,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
         <v>36</v>
@@ -986,7 +987,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49" t="s">
         <v>36</v>
@@ -994,18 +995,18 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" t="s">
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51" t="s">
         <v>3</v>
@@ -1013,34 +1014,34 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>